<commit_message>
add example of fetching multiple DHIS2 source (using Promise.all)
</commit_message>
<xml_diff>
--- a/hello-xlsx/data.xlsx
+++ b/hello-xlsx/data.xlsx
@@ -374,10 +374,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>code</v>
+      </c>
+      <c r="C1" t="str">
+        <v>name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
         <v>10</v>
       </c>
     </row>
@@ -387,11 +416,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>20</v>
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>code</v>
+      </c>
+      <c r="C1" t="str">
+        <v>name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -400,11 +458,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>30</v>
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>code</v>
+      </c>
+      <c r="C1" t="str">
+        <v>name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>